<commit_message>
Atualização 2º dia útil
</commit_message>
<xml_diff>
--- a/clientes_v2.xlsx
+++ b/clientes_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kantro-my.sharepoint.com/personal/faturamento_kantro_com_br/Documents/Documentos/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="234" documentId="8_{A4D66836-0EDD-4E4B-BE67-4B6397C4CDE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17F333C0-CE08-46AC-8D25-4F4D05BF541C}"/>
+  <xr:revisionPtr revIDLastSave="307" documentId="8_{A4D66836-0EDD-4E4B-BE67-4B6397C4CDE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B06C99F9-36FA-47BA-B2C8-5658A8A9C739}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{73EF806C-1D7D-472F-AA39-49083887D198}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="203">
   <si>
     <t>Tribunal de Justiça do Estado do Rio de Janeiro - TJ-RJ</t>
   </si>
@@ -647,6 +647,9 @@
   </si>
   <si>
     <t>09º Dia Útil</t>
+  </si>
+  <si>
+    <t>Em processamento</t>
   </si>
 </sst>
 </file>
@@ -1718,7 +1721,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M2">
-            <v>6179735.3666666672</v>
+            <v>6153878.7333333334</v>
           </cell>
           <cell r="N2">
             <v>775699</v>
@@ -1768,7 +1771,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M3">
-            <v>20466661.550000001</v>
+            <v>20444439.333333332</v>
           </cell>
           <cell r="N3">
             <v>666666.5</v>
@@ -1818,7 +1821,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M4">
-            <v>9031898.1263992023</v>
+            <v>9010696.4876048379</v>
           </cell>
           <cell r="N4">
             <v>636049.16383092967</v>
@@ -1868,7 +1871,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M5">
-            <v>3012858.4080000003</v>
+            <v>2994924.727</v>
           </cell>
           <cell r="N5">
             <v>538010.43000000005</v>
@@ -1918,7 +1921,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M6">
-            <v>3363881.6749999998</v>
+            <v>3349319.4166666665</v>
           </cell>
           <cell r="N6">
             <v>436867.75</v>
@@ -1968,7 +1971,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M7">
-            <v>2796804.4920000006</v>
+            <v>2782387.9740000004</v>
           </cell>
           <cell r="N7">
             <v>432495.54000000004</v>
@@ -2018,7 +2021,7 @@
             <v>Encerrado</v>
           </cell>
           <cell r="M8">
-            <v>0</v>
+            <v>-14382.223666666667</v>
           </cell>
           <cell r="N8">
             <v>431466.71</v>
@@ -2068,7 +2071,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M9">
-            <v>4225371.2659999998</v>
+            <v>4212449.6413333332</v>
           </cell>
           <cell r="N9">
             <v>387648.74</v>
@@ -2118,7 +2121,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M10">
-            <v>3758085.432</v>
+            <v>3746592.8160000001</v>
           </cell>
           <cell r="N10">
             <v>344778.48</v>
@@ -2168,7 +2171,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M11">
-            <v>897538.32</v>
+            <v>886319.0909999999</v>
           </cell>
           <cell r="N11">
             <v>336576.87</v>
@@ -2219,7 +2222,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M12">
-            <v>8833024.8579999991</v>
+            <v>8822279.0856666658</v>
           </cell>
           <cell r="N12">
             <v>322373.17</v>
@@ -2269,7 +2272,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M13">
-            <v>3331342.8020000001</v>
+            <v>3321155.2093333337</v>
           </cell>
           <cell r="N13">
             <v>305627.78000000003</v>
@@ -2319,7 +2322,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M14">
-            <v>1891083.4396666666</v>
+            <v>1880970.6939999999</v>
           </cell>
           <cell r="N14">
             <v>303382.37</v>
@@ -2369,7 +2372,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M15">
-            <v>3247732.1140000001</v>
+            <v>3238345.605</v>
           </cell>
           <cell r="N15">
             <v>281595.27</v>
@@ -2419,7 +2422,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M16">
-            <v>1801965.3903333331</v>
+            <v>1793425.2699999998</v>
           </cell>
           <cell r="N16">
             <v>256203.61</v>
@@ -2470,7 +2473,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M17">
-            <v>1535028.9219999998</v>
+            <v>1526776.0783333331</v>
           </cell>
           <cell r="N17">
             <v>247585.31</v>
@@ -2520,7 +2523,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M18">
-            <v>11148334.583333334</v>
+            <v>11141024.199999999</v>
           </cell>
           <cell r="N18">
             <v>219311.5</v>
@@ -2570,7 +2573,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M19">
-            <v>1160288.0916666666</v>
+            <v>1153081.3333333333</v>
           </cell>
           <cell r="N19">
             <v>216202.75</v>
@@ -2620,7 +2623,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M20">
-            <v>2340580.5583333336</v>
+            <v>2333378.7719999999</v>
           </cell>
           <cell r="N20">
             <v>216053.59</v>
@@ -2670,7 +2673,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M21">
-            <v>9129878.6400000006</v>
+            <v>9122734.7599999998</v>
           </cell>
           <cell r="N21">
             <v>214316.4</v>
@@ -2720,7 +2723,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M22">
-            <v>2316058.068</v>
+            <v>2309102.9386666669</v>
           </cell>
           <cell r="N22">
             <v>208653.88</v>
@@ -2770,7 +2773,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M23">
-            <v>1007580.2383333333</v>
+            <v>1001079.7206666666</v>
           </cell>
           <cell r="N23">
             <v>195015.53</v>
@@ -2820,7 +2823,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M24">
-            <v>202557.81333333335</v>
+            <v>196227.88166666668</v>
           </cell>
           <cell r="N24">
             <v>189897.95</v>
@@ -2870,7 +2873,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M25">
-            <v>1574578.0319999999</v>
+            <v>1569398.4989999998</v>
           </cell>
           <cell r="N25">
             <v>155385.99</v>
@@ -2920,7 +2923,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M26">
-            <v>719174.67466666654</v>
+            <v>714443.26233333326</v>
           </cell>
           <cell r="N26">
             <v>141942.37</v>
@@ -2971,7 +2974,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M27">
-            <v>987934.49399999995</v>
+            <v>983252.33999999985</v>
           </cell>
           <cell r="N27">
             <v>140464.62</v>
@@ -3021,7 +3024,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M28">
-            <v>990216.94933333329</v>
+            <v>985546.1146666666</v>
           </cell>
           <cell r="N28">
             <v>140125.04</v>
@@ -3071,7 +3074,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M29">
-            <v>582264.55700000003</v>
+            <v>577886.62800000003</v>
           </cell>
           <cell r="N29">
             <v>131337.87</v>
@@ -3121,7 +3124,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M30">
-            <v>821197.63199999998</v>
+            <v>816920.56099999999</v>
           </cell>
           <cell r="N30">
             <v>128312.13</v>
@@ -3171,7 +3174,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M31">
-            <v>1415888.2079999999</v>
+            <v>1411674.2549999999</v>
           </cell>
           <cell r="N31">
             <v>126418.59</v>
@@ -3215,7 +3218,7 @@
             <v>42522</v>
           </cell>
           <cell r="K32">
-            <v>45535</v>
+            <v>45536</v>
           </cell>
           <cell r="L32" t="str">
             <v>Vigente</v>
@@ -3271,7 +3274,7 @@
             <v>Encerrado</v>
           </cell>
           <cell r="M33">
-            <v>-66859.911999999997</v>
+            <v>-70792.847999999998</v>
           </cell>
           <cell r="N33">
             <v>117988.08</v>
@@ -3321,7 +3324,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M34">
-            <v>1079526.3170730164</v>
+            <v>1075790.931892833</v>
           </cell>
           <cell r="N34">
             <v>112061.55540550343</v>
@@ -3371,7 +3374,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M35">
-            <v>467502.39999999997</v>
+            <v>464385.71733333333</v>
           </cell>
           <cell r="N35">
             <v>93500.479999999996</v>
@@ -3421,7 +3424,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M36">
-            <v>428595.35666666663</v>
+            <v>425830.22533333331</v>
           </cell>
           <cell r="N36">
             <v>82953.94</v>
@@ -3471,7 +3474,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M37">
-            <v>410310.33600000001</v>
+            <v>408173.30299999996</v>
           </cell>
           <cell r="N37">
             <v>64110.99</v>
@@ -3521,7 +3524,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M38">
-            <v>332152.07999999996</v>
+            <v>330022.89999999997</v>
           </cell>
           <cell r="N38">
             <v>63875.4</v>
@@ -3571,7 +3574,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M39">
-            <v>321894.14999999997</v>
+            <v>319790.26666666666</v>
           </cell>
           <cell r="N39">
             <v>63116.5</v>
@@ -3615,7 +3618,7 @@
             <v>43525</v>
           </cell>
           <cell r="K40">
-            <v>45535</v>
+            <v>45536</v>
           </cell>
           <cell r="L40" t="str">
             <v>Vigente</v>
@@ -3671,7 +3674,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M41">
-            <v>471969.31400000001</v>
+            <v>470201.63866666669</v>
           </cell>
           <cell r="N41">
             <v>53030.26</v>
@@ -3721,7 +3724,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M42">
-            <v>264290.15999999997</v>
+            <v>262562.77333333332</v>
           </cell>
           <cell r="N42">
             <v>51821.599999999999</v>
@@ -3771,7 +3774,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M43">
-            <v>430236.07899999997</v>
+            <v>428660.12266666663</v>
           </cell>
           <cell r="N43">
             <v>47278.69</v>
@@ -3821,7 +3824,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M44">
-            <v>129125.70999999999</v>
+            <v>127606.584</v>
           </cell>
           <cell r="N44">
             <v>45573.78</v>
@@ -3871,7 +3874,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M45">
-            <v>218408.77500000002</v>
+            <v>216981.26666666669</v>
           </cell>
           <cell r="N45">
             <v>42825.25</v>
@@ -3921,7 +3924,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M46">
-            <v>214077.88833333334</v>
+            <v>212696.74066666668</v>
           </cell>
           <cell r="N46">
             <v>41434.43</v>
@@ -3972,7 +3975,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M47">
-            <v>251706.196</v>
+            <v>250466.264</v>
           </cell>
           <cell r="N47">
             <v>37197.96</v>
@@ -4022,7 +4025,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M48">
-            <v>180783.88533333331</v>
+            <v>179594.51766666665</v>
           </cell>
           <cell r="N48">
             <v>35681.03</v>
@@ -4072,7 +4075,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M49">
-            <v>272362.41666666669</v>
+            <v>271250.73333333334</v>
           </cell>
           <cell r="N49">
             <v>33350.5</v>
@@ -4122,7 +4125,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M50">
-            <v>165819.20699999999</v>
+            <v>164735.42133333333</v>
           </cell>
           <cell r="N50">
             <v>32513.57</v>
@@ -4173,7 +4176,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M51">
-            <v>153288.97165333334</v>
+            <v>152280.49157666668</v>
           </cell>
           <cell r="N51">
             <v>30254.402300000002</v>
@@ -4223,7 +4226,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M52">
-            <v>93832.271000000022</v>
+            <v>92864.928000000014</v>
           </cell>
           <cell r="N52">
             <v>29020.290000000005</v>
@@ -4267,7 +4270,7 @@
             <v>40969</v>
           </cell>
           <cell r="K53">
-            <v>45535</v>
+            <v>45536</v>
           </cell>
           <cell r="L53" t="str">
             <v>Vigente</v>
@@ -4317,7 +4320,7 @@
             <v>40186</v>
           </cell>
           <cell r="K54">
-            <v>45535</v>
+            <v>45536</v>
           </cell>
           <cell r="L54" t="str">
             <v>Vigente</v>
@@ -4367,7 +4370,7 @@
             <v>35555</v>
           </cell>
           <cell r="K55">
-            <v>45535</v>
+            <v>45536</v>
           </cell>
           <cell r="L55" t="str">
             <v>Vigente</v>
@@ -4417,7 +4420,7 @@
             <v>42653</v>
           </cell>
           <cell r="K56">
-            <v>45535</v>
+            <v>45536</v>
           </cell>
           <cell r="L56" t="str">
             <v>Vigente</v>
@@ -4473,7 +4476,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M57">
-            <v>332305.95199999999</v>
+            <v>331808.48800000001</v>
           </cell>
           <cell r="N57">
             <v>14923.92</v>
@@ -4523,7 +4526,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M58">
-            <v>181105.70599999998</v>
+            <v>180610.88166666665</v>
           </cell>
           <cell r="N58">
             <v>14844.73</v>
@@ -4573,7 +4576,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M59">
-            <v>73797.101666666655</v>
+            <v>73320.991333333324</v>
           </cell>
           <cell r="N59">
             <v>14283.31</v>
@@ -4614,10 +4617,10 @@
             <v>-</v>
           </cell>
           <cell r="J60">
-            <v>45505</v>
+            <v>45506</v>
           </cell>
           <cell r="K60">
-            <v>45535</v>
+            <v>45536</v>
           </cell>
           <cell r="L60" t="str">
             <v>Vigente</v>
@@ -4661,13 +4664,13 @@
             <v>Rua Monsenhor Manuel Gomes, 370 - São Cristóvão, Rio de Janeiro - RJ</v>
           </cell>
           <cell r="I61">
-            <v>45505</v>
+            <v>45506</v>
           </cell>
           <cell r="J61">
             <v>43466</v>
           </cell>
           <cell r="K61">
-            <v>45535</v>
+            <v>45536</v>
           </cell>
           <cell r="L61" t="str">
             <v>Vigente</v>
@@ -4723,7 +4726,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M62">
-            <v>78537.666666666672</v>
+            <v>78311.333333333343</v>
           </cell>
           <cell r="N62">
             <v>6790</v>
@@ -4731,6 +4734,7 @@
           <cell r="O62" t="str">
             <v>Insetkan</v>
           </cell>
+          <cell r="P62"/>
         </row>
         <row r="63">
           <cell r="A63" t="str">
@@ -4770,7 +4774,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M63">
-            <v>39576.274000000005</v>
+            <v>39363.498333333337</v>
           </cell>
           <cell r="N63">
             <v>6383.27</v>
@@ -4820,7 +4824,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M64">
-            <v>154967.345</v>
+            <v>154788.19199999998</v>
           </cell>
           <cell r="N64">
             <v>5374.59</v>
@@ -4828,6 +4832,7 @@
           <cell r="O64" t="str">
             <v>Insetkan</v>
           </cell>
+          <cell r="P64"/>
         </row>
         <row r="65">
           <cell r="A65" t="str">
@@ -4867,7 +4872,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M65">
-            <v>18720.54</v>
+            <v>18581.869333333336</v>
           </cell>
           <cell r="N65">
             <v>4160.12</v>
@@ -4917,7 +4922,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M66">
-            <v>10467.453333333333</v>
+            <v>10369.626666666667</v>
           </cell>
           <cell r="N66">
             <v>2934.8</v>
@@ -4925,6 +4930,7 @@
           <cell r="O66" t="str">
             <v>Insetkan</v>
           </cell>
+          <cell r="P66"/>
         </row>
         <row r="67">
           <cell r="A67" t="str">
@@ -4964,7 +4970,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M67">
-            <v>7561.3333333333339</v>
+            <v>7490.666666666667</v>
           </cell>
           <cell r="N67">
             <v>2120</v>
@@ -4972,6 +4978,7 @@
           <cell r="O67" t="str">
             <v>Insetkan</v>
           </cell>
+          <cell r="P67"/>
         </row>
         <row r="68">
           <cell r="A68" t="str">
@@ -5011,7 +5018,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M68">
-            <v>4574.6666666666661</v>
+            <v>4512</v>
           </cell>
           <cell r="N68">
             <v>1880</v>
@@ -5019,6 +5026,7 @@
           <cell r="O68" t="str">
             <v>Insetkan</v>
           </cell>
+          <cell r="P68"/>
         </row>
         <row r="69">
           <cell r="A69" t="str">
@@ -5058,7 +5066,7 @@
             <v>Vigente</v>
           </cell>
           <cell r="M69">
-            <v>4830.0533333333333</v>
+            <v>4798.2766666666666</v>
           </cell>
           <cell r="N69">
             <v>953.3</v>
@@ -5102,7 +5110,7 @@
             <v>43828</v>
           </cell>
           <cell r="K70">
-            <v>45535</v>
+            <v>45536</v>
           </cell>
           <cell r="L70" t="str">
             <v>Vigente</v>
@@ -5121,7 +5129,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -5479,25 +5487,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06736F0B-1E7B-40B2-AFB2-0995320CCBFA}">
   <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24" style="1" customWidth="1" outlineLevel="1"/>
     <col min="2" max="2" width="62.85546875" style="6" customWidth="1"/>
     <col min="3" max="3" width="26" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="27.7109375" style="2" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="26.7109375" style="2" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="27.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="20.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="28" style="6" customWidth="1"/>
     <col min="8" max="8" width="30.7109375" style="3" customWidth="1" outlineLevel="1"/>
     <col min="9" max="9" width="20.42578125" style="3" customWidth="1" outlineLevel="1"/>
     <col min="10" max="10" width="28" style="3" customWidth="1" outlineLevel="1"/>
     <col min="11" max="11" width="30.28515625" style="6" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="24.5703125" style="6" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="9.140625" style="6"/>
+    <col min="12" max="12" width="24.5703125" style="6" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="6" customWidth="1" outlineLevel="1"/>
     <col min="14" max="14" width="77.140625" style="6" customWidth="1" outlineLevel="1"/>
     <col min="15" max="16384" width="9.140625" style="6"/>
   </cols>
@@ -5568,7 +5574,7 @@
         <v>192</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>169</v>
+        <v>202</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>61</v>
@@ -5616,7 +5622,7 @@
         <v>192</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>64</v>
@@ -5762,7 +5768,7 @@
         <v>192</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>71</v>
@@ -6399,7 +6405,7 @@
         <v>192</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>93</v>
@@ -6486,17 +6492,17 @@
       </c>
       <c r="D21" s="33" t="str">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO","A ser apurado",IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan","Insetkan","Apurado"))</f>
-        <v>A ser apurado</v>
+        <v>Apurado</v>
       </c>
       <c r="E21" s="10">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO",0,IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan",0,Tabela1[[#This Row],[Faturar Após Medição]]))</f>
-        <v>0</v>
+        <v>214316.4</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>192</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>95</v>
@@ -6511,9 +6517,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>Vigente</v>
       </c>
-      <c r="L21" s="11" t="str">
-        <f>VLOOKUP(Tabela1[[#This Row],[Chave]],'[1]07.2024'!$A$1:$P$70,15,0)</f>
-        <v>A ser apurado</v>
+      <c r="L21" s="11">
+        <v>214316.4</v>
       </c>
       <c r="M21" s="7" t="s">
         <v>187</v>
@@ -6643,7 +6648,7 @@
         <v>192</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>169</v>
+        <v>202</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>101</v>
@@ -7270,17 +7275,17 @@
       </c>
       <c r="D37" s="33" t="str">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO","A ser apurado",IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan","Insetkan","Apurado"))</f>
-        <v>A ser apurado</v>
+        <v>Apurado</v>
       </c>
       <c r="E37" s="10">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO",0,IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan",0,Tabela1[[#This Row],[Faturar Após Medição]]))</f>
-        <v>0</v>
+        <v>64110.99</v>
       </c>
       <c r="F37" s="10" t="s">
         <v>197</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>174</v>
+        <v>202</v>
       </c>
       <c r="H37" s="7" t="s">
         <v>122</v>
@@ -7295,9 +7300,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>Vigente</v>
       </c>
-      <c r="L37" s="31" t="str">
-        <f>VLOOKUP(Tabela1[[#This Row],[Chave]],'[1]07.2024'!$A$1:$P$70,15,0)</f>
-        <v>A ser apurado</v>
+      <c r="L37" s="31">
+        <v>64110.99</v>
       </c>
       <c r="M37" s="7" t="s">
         <v>187</v>
@@ -7368,17 +7372,17 @@
       </c>
       <c r="D39" s="33" t="str">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO","A ser apurado",IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan","Insetkan","Apurado"))</f>
-        <v>A ser apurado</v>
+        <v>Apurado</v>
       </c>
       <c r="E39" s="10">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO",0,IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan",0,Tabela1[[#This Row],[Faturar Após Medição]]))</f>
-        <v>0</v>
+        <v>63116.5</v>
       </c>
       <c r="F39" s="10" t="s">
         <v>197</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>174</v>
+        <v>202</v>
       </c>
       <c r="H39" s="7" t="s">
         <v>122</v>
@@ -7393,9 +7397,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>Vigente</v>
       </c>
-      <c r="L39" s="31" t="str">
-        <f>VLOOKUP(Tabela1[[#This Row],[Chave]],'[1]07.2024'!$A$1:$P$70,15,0)</f>
-        <v>A ser apurado</v>
+      <c r="L39" s="31">
+        <v>63116.5</v>
       </c>
       <c r="M39" s="7" t="s">
         <v>187</v>
@@ -7760,17 +7763,17 @@
       </c>
       <c r="D47" s="33" t="str">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO","A ser apurado",IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan","Insetkan","Apurado"))</f>
-        <v>A ser apurado</v>
+        <v>Apurado</v>
       </c>
       <c r="E47" s="10">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO",0,IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan",0,Tabela1[[#This Row],[Faturar Após Medição]]))</f>
-        <v>0</v>
+        <v>37197.96</v>
       </c>
       <c r="F47" s="10" t="s">
         <v>197</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>174</v>
+        <v>202</v>
       </c>
       <c r="H47" s="7" t="s">
         <v>139</v>
@@ -7785,9 +7788,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>Vigente</v>
       </c>
-      <c r="L47" s="31" t="str">
-        <f>VLOOKUP(Tabela1[[#This Row],[Chave]],'[1]07.2024'!$A$1:$P$70,15,0)</f>
-        <v>A ser apurado</v>
+      <c r="L47" s="31">
+        <v>37197.96</v>
       </c>
       <c r="M47" s="7" t="s">
         <v>188</v>
@@ -8942,12 +8944,18 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1F18F452-72E2-41F2-BB8E-C375E17331F1}">
           <x14:formula1>
             <xm:f>Planilha2!$A$2:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G70</xm:sqref>
+          <xm:sqref>G3:G70</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C888B976-EE8D-40D9-8ED3-8BBDBF9BDF75}">
+          <x14:formula1>
+            <xm:f>Planilha2!$A$2:$A$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -8957,10 +8965,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06655113-8824-4D66-AF55-7F00CA308594}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8975,36 +8983,41 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>173</v>
       </c>
     </row>

</xml_diff>

<commit_message>
atualização segundo dia útil
</commit_message>
<xml_diff>
--- a/clientes_v2.xlsx
+++ b/clientes_v2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kantro-my.sharepoint.com/personal/faturamento_kantro_com_br/Documents/Documentos/Python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Faturamento\OneDrive - GRUPO KANTRO\Documentos\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="408" documentId="8_{A4D66836-0EDD-4E4B-BE67-4B6397C4CDE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A3C42D1-D35C-42D2-A310-C89EB9826905}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A221F788-C7DD-432B-A126-A446701B8034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{73EF806C-1D7D-472F-AA39-49083887D198}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="192">
   <si>
     <t>Tribunal de Justiça do Estado do Rio de Janeiro - TJ-RJ</t>
   </si>
@@ -201,22 +201,10 @@
     <t>MSC Mediterranean Ltda</t>
   </si>
   <si>
-    <t>Instituto Federal de Educação RJ – IFRJ Campus Volta Redonda</t>
-  </si>
-  <si>
     <t>Serviço Social do Comércio - Departamento Nacional - Sesc DN</t>
   </si>
   <si>
     <t>Banco da Providência</t>
-  </si>
-  <si>
-    <t>Serviço Social do Comércio - Polo Sociocultural Sesc Paraty</t>
-  </si>
-  <si>
-    <t>Serviço Social do Comércio - Departamento Nacional</t>
-  </si>
-  <si>
-    <t>Serviço Nacional de Aprendizagem Industrial - SENAI-CETIQT</t>
   </si>
   <si>
     <t>Fundação Cultural do Exército Brasileiro - FUNCEB</t>
@@ -508,33 +496,15 @@
     <t>Ipanema - Rio de Janeiro</t>
   </si>
   <si>
-    <t>Controle de Pragas e Vetores</t>
-  </si>
-  <si>
-    <t>Volta Redonda - RJ</t>
-  </si>
-  <si>
     <t>21D_0023-PG</t>
   </si>
   <si>
-    <t>2021.7421.5355</t>
-  </si>
-  <si>
     <t>Realengo - Rio de Janeiro</t>
   </si>
   <si>
-    <t>Paraty - RJ</t>
-  </si>
-  <si>
-    <t>Jacarepaguá - RJ</t>
-  </si>
-  <si>
     <t>Limpeza Expressa</t>
   </si>
   <si>
-    <t>Insetkan</t>
-  </si>
-  <si>
     <t>Nome Prestador</t>
   </si>
   <si>
@@ -608,9 +578,6 @@
   </si>
   <si>
     <t>KT</t>
-  </si>
-  <si>
-    <t>INSET</t>
   </si>
   <si>
     <t>Chave</t>
@@ -4734,6 +4701,7 @@
           <cell r="O62" t="str">
             <v>Insetkan</v>
           </cell>
+          <cell r="P62"/>
         </row>
         <row r="63">
           <cell r="A63" t="str">
@@ -4831,6 +4799,7 @@
           <cell r="O64" t="str">
             <v>Insetkan</v>
           </cell>
+          <cell r="P64"/>
         </row>
         <row r="65">
           <cell r="A65" t="str">
@@ -4928,6 +4897,7 @@
           <cell r="O66" t="str">
             <v>Insetkan</v>
           </cell>
+          <cell r="P66"/>
         </row>
         <row r="67">
           <cell r="A67" t="str">
@@ -4975,6 +4945,7 @@
           <cell r="O67" t="str">
             <v>Insetkan</v>
           </cell>
+          <cell r="P67"/>
         </row>
         <row r="68">
           <cell r="A68" t="str">
@@ -5022,6 +4993,7 @@
           <cell r="O68" t="str">
             <v>Insetkan</v>
           </cell>
+          <cell r="P68"/>
         </row>
         <row r="69">
           <cell r="A69" t="str">
@@ -5124,15 +5096,15 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{26494283-FBA1-4516-934A-E8D02932BB12}" name="Tabela1" displayName="Tabela1" ref="A1:N70" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" headerRowCellStyle="Moeda">
-  <autoFilter ref="A1:N70" xr:uid="{26494283-FBA1-4516-934A-E8D02932BB12}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{26494283-FBA1-4516-934A-E8D02932BB12}" name="Tabela1" displayName="Tabela1" ref="A1:N65" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" headerRowCellStyle="Moeda">
+  <autoFilter ref="A1:N65" xr:uid="{26494283-FBA1-4516-934A-E8D02932BB12}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{A5031065-3A63-4E12-A452-CE124BCAE36D}" name="Nome Prestador" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{5B3E423B-A53E-4066-A892-BA5BA864FF7E}" name="Razão Social do Tomador" dataDxfId="14"/>
@@ -5480,9 +5452,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06736F0B-1E7B-40B2-AFB2-0995320CCBFA}">
-  <dimension ref="A1:N70"/>
+  <dimension ref="A1:N65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5505,51 +5479,51 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="G1" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="N1" s="5" t="s">
         <v>179</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>0</v>
@@ -5566,19 +5540,19 @@
         <v>576558.80827391299</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="K2" s="9" t="str">
         <f ca="1">IF(J2&gt;TODAY(),"Vigente","Encerrado")</f>
@@ -5588,7 +5562,7 @@
         <v>576558.80827391299</v>
       </c>
       <c r="M2" s="27" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N2" s="39" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -5597,7 +5571,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>1</v>
@@ -5614,22 +5588,22 @@
         <v>610366.98</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="K3" s="9" t="str">
-        <f t="shared" ref="K3:K66" ca="1" si="0">IF(J3&gt;TODAY(),"Vigente","Encerrado")</f>
+        <f t="shared" ref="K3:K63" ca="1" si="0">IF(J3&gt;TODAY(),"Vigente","Encerrado")</f>
         <v>Vigente</v>
       </c>
       <c r="L3" s="11">
@@ -5637,7 +5611,7 @@
         <v>610366.98</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N3" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -5646,7 +5620,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>2</v>
@@ -5663,19 +5637,19 @@
         <v>579885.07999999996</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="H4" s="7">
         <v>8000013262</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="K4" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -5685,7 +5659,7 @@
         <v>579885.07999999996</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N4" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -5694,7 +5668,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>3</v>
@@ -5711,19 +5685,19 @@
         <v>0</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K5" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -5734,7 +5708,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N5" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -5743,7 +5717,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>4</v>
@@ -5760,19 +5734,19 @@
         <v>436867.75</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K6" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -5783,7 +5757,7 @@
         <v>436867.75</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N6" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -5792,7 +5766,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>5</v>
@@ -5809,19 +5783,19 @@
         <v>0</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K7" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -5832,7 +5806,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N7" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -5841,7 +5815,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>6</v>
@@ -5858,19 +5832,19 @@
         <v>0</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="K8" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -5881,7 +5855,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N8" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -5890,7 +5864,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>5</v>
@@ -5907,19 +5881,19 @@
         <v>0</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K9" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -5930,7 +5904,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N9" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -5939,7 +5913,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>5</v>
@@ -5956,19 +5930,19 @@
         <v>0</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K10" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -5979,7 +5953,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N10" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -5988,7 +5962,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>5</v>
@@ -6005,19 +5979,19 @@
         <v>0</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K11" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -6028,7 +6002,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N11" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -6037,7 +6011,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>7</v>
@@ -6054,19 +6028,19 @@
         <v>0</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K12" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -6077,7 +6051,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N12" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -6086,7 +6060,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>5</v>
@@ -6103,19 +6077,19 @@
         <v>0</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K13" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -6126,7 +6100,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N13" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -6135,7 +6109,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>5</v>
@@ -6152,19 +6126,19 @@
         <v>0</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="K14" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -6175,7 +6149,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N14" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -6184,7 +6158,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>8</v>
@@ -6201,19 +6175,19 @@
         <v>0</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="K15" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -6224,7 +6198,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N15" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -6233,7 +6207,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>9</v>
@@ -6250,19 +6224,19 @@
         <v>0</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K16" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -6273,7 +6247,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N16" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -6282,7 +6256,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>10</v>
@@ -6299,19 +6273,19 @@
         <v>246203.6</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K17" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -6321,7 +6295,7 @@
         <v>246203.6</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N17" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -6330,7 +6304,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>11</v>
@@ -6347,19 +6321,19 @@
         <v>0</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="K18" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -6370,7 +6344,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M18" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N18" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -6379,7 +6353,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>12</v>
@@ -6396,19 +6370,19 @@
         <v>228186.31</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="K19" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -6418,7 +6392,7 @@
         <v>228186.31</v>
       </c>
       <c r="M19" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N19" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -6427,7 +6401,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>13</v>
@@ -6444,19 +6418,19 @@
         <v>216053.59</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="K20" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -6467,7 +6441,7 @@
         <v>216053.59</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N20" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -6476,7 +6450,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>14</v>
@@ -6493,19 +6467,19 @@
         <v>214316.4</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K21" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -6515,7 +6489,7 @@
         <v>214316.4</v>
       </c>
       <c r="M21" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N21" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -6524,7 +6498,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>15</v>
@@ -6541,19 +6515,19 @@
         <v>0</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="K22" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -6564,7 +6538,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N22" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -6573,7 +6547,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>10</v>
@@ -6590,19 +6564,19 @@
         <v>191173.65546394369</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K23" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -6612,7 +6586,7 @@
         <v>191173.65546394369</v>
       </c>
       <c r="M23" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N23" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -6621,7 +6595,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>16</v>
@@ -6638,19 +6612,19 @@
         <v>189897.95</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K24" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -6661,7 +6635,7 @@
         <v>189897.95</v>
       </c>
       <c r="M24" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N24" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -6670,7 +6644,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>3</v>
@@ -6687,19 +6661,19 @@
         <v>0</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K25" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -6710,7 +6684,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M25" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N25" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -6719,7 +6693,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>17</v>
@@ -6729,37 +6703,36 @@
       </c>
       <c r="D26" s="33" t="str">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO","A ser apurado",IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan","Insetkan","Apurado"))</f>
-        <v>A ser apurado</v>
+        <v>Apurado</v>
       </c>
       <c r="E26" s="10">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO",0,IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan",0,Tabela1[[#This Row],[Faturar Após Medição]]))</f>
-        <v>0</v>
+        <v>141942.37</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="K26" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>Vigente</v>
       </c>
-      <c r="L26" s="11" t="str">
-        <f>VLOOKUP(Tabela1[[#This Row],[Chave]],'[1]07.2024'!$A$1:$P$70,15,0)</f>
-        <v>A ser apurado</v>
+      <c r="L26" s="11">
+        <v>141942.37</v>
       </c>
       <c r="M26" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N26" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -6768,7 +6741,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>18</v>
@@ -6785,19 +6758,19 @@
         <v>0</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K27" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -6808,7 +6781,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M27" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N27" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -6817,7 +6790,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B28" s="13" t="s">
         <v>19</v>
@@ -6834,19 +6807,19 @@
         <v>0</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I28" s="12" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J28" s="12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K28" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -6857,7 +6830,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M28" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N28" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -6866,7 +6839,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B29" s="18" t="s">
         <v>20</v>
@@ -6883,19 +6856,19 @@
         <v>0</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I29" s="17" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J29" s="17" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K29" s="19" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -6906,7 +6879,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M29" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N29" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -6915,7 +6888,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B30" s="23" t="s">
         <v>21</v>
@@ -6932,19 +6905,19 @@
         <v>0</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H30" s="22" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I30" s="22" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="J30" s="22" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K30" s="24" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -6955,7 +6928,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M30" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N30" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -6964,7 +6937,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B31" s="28" t="s">
         <v>22</v>
@@ -6981,19 +6954,19 @@
         <v>0</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H31" s="27" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="I31" s="27" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J31" s="27" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K31" s="29" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -7004,7 +6977,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M31" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N31" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -7013,7 +6986,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>23</v>
@@ -7030,19 +7003,19 @@
         <v>118243.07</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="K32" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -7053,7 +7026,7 @@
         <v>118243.07</v>
       </c>
       <c r="M32" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N32" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -7062,7 +7035,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>24</v>
@@ -7079,19 +7052,19 @@
         <v>58090.33</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="K33" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -7102,7 +7075,7 @@
         <v>58090.33</v>
       </c>
       <c r="M33" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N33" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -7111,7 +7084,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>25</v>
@@ -7128,19 +7101,19 @@
         <v>0</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K34" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -7151,7 +7124,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M34" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N34" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -7160,7 +7133,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>26</v>
@@ -7177,19 +7150,19 @@
         <v>0</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K35" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -7200,7 +7173,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M35" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N35" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -7209,7 +7182,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>27</v>
@@ -7219,37 +7192,36 @@
       </c>
       <c r="D36" s="33" t="str">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO","A ser apurado",IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan","Insetkan","Apurado"))</f>
-        <v>A ser apurado</v>
+        <v>Apurado</v>
       </c>
       <c r="E36" s="10">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO",0,IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan",0,Tabela1[[#This Row],[Faturar Após Medição]]))</f>
-        <v>0</v>
+        <v>82953.94</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K36" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>Vigente</v>
       </c>
-      <c r="L36" s="31" t="str">
-        <f>VLOOKUP(Tabela1[[#This Row],[Chave]],'[1]07.2024'!$A$1:$P$70,15,0)</f>
-        <v>A ser apurado</v>
+      <c r="L36" s="31">
+        <v>82953.94</v>
       </c>
       <c r="M36" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N36" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -7258,7 +7230,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>28</v>
@@ -7275,19 +7247,19 @@
         <v>64110.99</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>202</v>
+        <v>158</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="K37" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -7297,7 +7269,7 @@
         <v>64110.99</v>
       </c>
       <c r="M37" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N37" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -7306,7 +7278,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>29</v>
@@ -7323,19 +7295,19 @@
         <v>0</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="K38" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -7346,7 +7318,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M38" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N38" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -7355,7 +7327,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>30</v>
@@ -7372,19 +7344,19 @@
         <v>63116.5</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>202</v>
+        <v>158</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K39" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -7394,7 +7366,7 @@
         <v>63116.5</v>
       </c>
       <c r="M39" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N39" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -7403,7 +7375,7 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>31</v>
@@ -7420,19 +7392,19 @@
         <v>0</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="J40" s="7" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="K40" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -7443,7 +7415,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M40" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N40" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -7452,7 +7424,7 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>32</v>
@@ -7469,19 +7441,19 @@
         <v>0</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J41" s="7" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="K41" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -7492,7 +7464,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M41" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N41" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -7501,7 +7473,7 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>33</v>
@@ -7511,37 +7483,36 @@
       </c>
       <c r="D42" s="33" t="str">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO","A ser apurado",IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan","Insetkan","Apurado"))</f>
-        <v>A ser apurado</v>
+        <v>Apurado</v>
       </c>
       <c r="E42" s="10">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO",0,IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan",0,Tabela1[[#This Row],[Faturar Após Medição]]))</f>
-        <v>0</v>
+        <v>51821.599999999999</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J42" s="7" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="K42" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>Vigente</v>
       </c>
-      <c r="L42" s="31" t="str">
-        <f>VLOOKUP(Tabela1[[#This Row],[Chave]],'[1]07.2024'!$A$1:$P$70,15,0)</f>
-        <v>A ser apurado</v>
+      <c r="L42" s="31">
+        <v>51821.599999999999</v>
       </c>
       <c r="M42" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N42" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -7550,7 +7521,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>34</v>
@@ -7567,19 +7538,19 @@
         <v>0</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J43" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="K43" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -7590,7 +7561,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M43" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N43" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -7599,7 +7570,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>35</v>
@@ -7616,19 +7587,19 @@
         <v>0</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="J44" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="K44" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -7639,7 +7610,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M44" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N44" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -7648,7 +7619,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>36</v>
@@ -7658,37 +7629,36 @@
       </c>
       <c r="D45" s="33" t="str">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO","A ser apurado",IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan","Insetkan","Apurado"))</f>
-        <v>A ser apurado</v>
+        <v>Apurado</v>
       </c>
       <c r="E45" s="10">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO",0,IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan",0,Tabela1[[#This Row],[Faturar Após Medição]]))</f>
-        <v>0</v>
+        <v>42825.25</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J45" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K45" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>Vigente</v>
       </c>
-      <c r="L45" s="31" t="str">
-        <f>VLOOKUP(Tabela1[[#This Row],[Chave]],'[1]07.2024'!$A$1:$P$70,15,0)</f>
-        <v>A ser apurado</v>
+      <c r="L45" s="31">
+        <v>42825.25</v>
       </c>
       <c r="M45" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N45" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -7697,7 +7667,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>37</v>
@@ -7707,37 +7677,36 @@
       </c>
       <c r="D46" s="33" t="str">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO","A ser apurado",IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan","Insetkan","Apurado"))</f>
-        <v>A ser apurado</v>
+        <v>Apurado</v>
       </c>
       <c r="E46" s="10">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO",0,IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan",0,Tabela1[[#This Row],[Faturar Após Medição]]))</f>
-        <v>0</v>
+        <v>41434.43</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J46" s="7" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K46" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>Vigente</v>
       </c>
-      <c r="L46" s="31" t="str">
-        <f>VLOOKUP(Tabela1[[#This Row],[Chave]],'[1]07.2024'!$A$1:$P$70,15,0)</f>
-        <v>A ser apurado</v>
+      <c r="L46" s="31">
+        <v>41434.43</v>
       </c>
       <c r="M46" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N46" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -7746,7 +7715,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>38</v>
@@ -7763,19 +7732,19 @@
         <v>37197.96</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J47" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K47" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -7785,7 +7754,7 @@
         <v>37197.96</v>
       </c>
       <c r="M47" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N47" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -7794,7 +7763,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>39</v>
@@ -7804,37 +7773,36 @@
       </c>
       <c r="D48" s="33" t="str">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO","A ser apurado",IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan","Insetkan","Apurado"))</f>
-        <v>A ser apurado</v>
+        <v>Apurado</v>
       </c>
       <c r="E48" s="10">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO",0,IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan",0,Tabela1[[#This Row],[Faturar Após Medição]]))</f>
-        <v>0</v>
+        <v>35681.03</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J48" s="7" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="K48" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>Vigente</v>
       </c>
-      <c r="L48" s="31" t="str">
-        <f>VLOOKUP(Tabela1[[#This Row],[Chave]],'[1]07.2024'!$A$1:$P$70,15,0)</f>
-        <v>A ser apurado</v>
+      <c r="L48" s="31">
+        <v>35681.03</v>
       </c>
       <c r="M48" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N48" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -7843,7 +7811,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>40</v>
@@ -7860,19 +7828,19 @@
         <v>0</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J49" s="7" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="K49" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -7883,7 +7851,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M49" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N49" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -7892,7 +7860,7 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>41</v>
@@ -7902,37 +7870,36 @@
       </c>
       <c r="D50" s="33" t="str">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO","A ser apurado",IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan","Insetkan","Apurado"))</f>
-        <v>A ser apurado</v>
+        <v>Apurado</v>
       </c>
       <c r="E50" s="10">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO",0,IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan",0,Tabela1[[#This Row],[Faturar Após Medição]]))</f>
-        <v>0</v>
+        <v>32513.57</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I50" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J50" s="7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="K50" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>Vigente</v>
       </c>
-      <c r="L50" s="31" t="str">
-        <f>VLOOKUP(Tabela1[[#This Row],[Chave]],'[1]07.2024'!$A$1:$P$70,15,0)</f>
-        <v>A ser apurado</v>
+      <c r="L50" s="31">
+        <v>32513.57</v>
       </c>
       <c r="M50" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N50" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -7941,7 +7908,7 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>42</v>
@@ -7951,37 +7918,36 @@
       </c>
       <c r="D51" s="33" t="str">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO","A ser apurado",IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan","Insetkan","Apurado"))</f>
-        <v>A ser apurado</v>
+        <v>Apurado</v>
       </c>
       <c r="E51" s="10">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO",0,IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan",0,Tabela1[[#This Row],[Faturar Após Medição]]))</f>
-        <v>0</v>
+        <v>30254.402300000002</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J51" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K51" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>Vigente</v>
       </c>
-      <c r="L51" s="31" t="str">
-        <f>VLOOKUP(Tabela1[[#This Row],[Chave]],'[1]07.2024'!$A$1:$P$70,15,0)</f>
-        <v>A ser apurado</v>
+      <c r="L51" s="31">
+        <v>30254.402300000002</v>
       </c>
       <c r="M51" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N51" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -7990,7 +7956,7 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>43</v>
@@ -8000,37 +7966,36 @@
       </c>
       <c r="D52" s="33" t="str">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO","A ser apurado",IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan","Insetkan","Apurado"))</f>
-        <v>A ser apurado</v>
+        <v>Apurado</v>
       </c>
       <c r="E52" s="10">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO",0,IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan",0,Tabela1[[#This Row],[Faturar Após Medição]]))</f>
-        <v>0</v>
+        <v>29020.290000000005</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J52" s="7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="K52" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>Vigente</v>
       </c>
-      <c r="L52" s="31" t="str">
-        <f>VLOOKUP(Tabela1[[#This Row],[Chave]],'[1]07.2024'!$A$1:$P$70,15,0)</f>
-        <v>A ser apurado</v>
+      <c r="L52" s="31">
+        <v>29020.290000000005</v>
       </c>
       <c r="M52" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N52" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -8039,7 +8004,7 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>44</v>
@@ -8056,19 +8021,19 @@
         <v>0</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J53" s="7" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K53" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -8079,7 +8044,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M53" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N53" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -8088,7 +8053,7 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>45</v>
@@ -8105,19 +8070,19 @@
         <v>0</v>
       </c>
       <c r="F54" s="10" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I54" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="J54" s="7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K54" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -8128,7 +8093,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M54" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N54" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -8137,7 +8102,7 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>46</v>
@@ -8154,19 +8119,19 @@
         <v>0</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J55" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="K55" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -8177,7 +8142,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M55" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N55" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -8186,7 +8151,7 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>47</v>
@@ -8203,19 +8168,19 @@
         <v>0</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I56" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J56" s="7" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K56" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -8226,7 +8191,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M56" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N56" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -8235,7 +8200,7 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>48</v>
@@ -8252,19 +8217,19 @@
         <v>0</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J57" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K57" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -8275,7 +8240,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M57" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N57" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -8284,7 +8249,7 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>49</v>
@@ -8301,19 +8266,19 @@
         <v>0</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I58" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J58" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K58" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -8324,7 +8289,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M58" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N58" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -8333,7 +8298,7 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>50</v>
@@ -8350,19 +8315,19 @@
         <v>0</v>
       </c>
       <c r="F59" s="10" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="I59" s="7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="J59" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="K59" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -8373,7 +8338,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M59" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N59" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -8382,7 +8347,7 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>51</v>
@@ -8399,19 +8364,19 @@
         <v>0</v>
       </c>
       <c r="F60" s="10" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I60" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J60" s="7" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="K60" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -8422,7 +8387,7 @@
         <v>A ser apurado</v>
       </c>
       <c r="M60" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="N60" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -8431,7 +8396,7 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="32" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>52</v>
@@ -8448,19 +8413,19 @@
         <v>9588.7800000000007</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I61" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J61" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K61" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -8471,7 +8436,7 @@
         <v>9588.7800000000007</v>
       </c>
       <c r="M61" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="N61" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
@@ -8480,36 +8445,36 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="32" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C62" s="10">
-        <v>6790</v>
+        <v>6383.27</v>
       </c>
       <c r="D62" s="33" t="str">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO","A ser apurado",IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan","Insetkan","Apurado"))</f>
-        <v>Insetkan</v>
+        <v>A ser apurado</v>
       </c>
       <c r="E62" s="10">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO",0,IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan",0,Tabela1[[#This Row],[Faturar Após Medição]]))</f>
         <v>0</v>
       </c>
       <c r="F62" s="10" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="G62" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H62" s="7" t="s">
         <v>151</v>
       </c>
       <c r="I62" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="J62" s="7" t="s">
-        <v>156</v>
+        <v>68</v>
       </c>
       <c r="K62" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -8517,416 +8482,171 @@
       </c>
       <c r="L62" s="31" t="str">
         <f>VLOOKUP(Tabela1[[#This Row],[Chave]],'[1]07.2024'!$A$1:$P$70,15,0)</f>
-        <v>Insetkan</v>
+        <v>A ser apurado</v>
       </c>
       <c r="M62" s="7" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="N62" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
-        <v>INSET_Instituto Federal de Educação RJ – IFRJ Campus Volta Redonda_Controle de Pragas e Vetores</v>
+        <v>KT_Serviço Social do Comércio - Departamento Nacional - Sesc DN_Motoboy</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="32" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>54</v>
       </c>
       <c r="C63" s="10">
-        <v>6383.27</v>
+        <v>4160.12</v>
       </c>
       <c r="D63" s="33" t="str">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO","A ser apurado",IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan","Insetkan","Apurado"))</f>
-        <v>A ser apurado</v>
+        <v>Apurado</v>
       </c>
       <c r="E63" s="10">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO",0,IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan",0,Tabela1[[#This Row],[Faturar Após Medição]]))</f>
-        <v>0</v>
+        <v>4160.12</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>157</v>
+        <v>109</v>
       </c>
       <c r="I63" s="7" t="s">
-        <v>150</v>
+        <v>74</v>
       </c>
       <c r="J63" s="7" t="s">
-        <v>72</v>
+        <v>152</v>
       </c>
       <c r="K63" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>Vigente</v>
       </c>
-      <c r="L63" s="31" t="str">
+      <c r="L63" s="11">
         <f>VLOOKUP(Tabela1[[#This Row],[Chave]],'[1]07.2024'!$A$1:$P$70,15,0)</f>
-        <v>A ser apurado</v>
+        <v>4160.12</v>
       </c>
       <c r="M63" s="7" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="N63" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
-        <v>KT_Serviço Social do Comércio - Departamento Nacional - Sesc DN_Motoboy</v>
+        <v xml:space="preserve">KE_Banco da Providência_Limpeza </v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="32" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="C64" s="10">
-        <v>5374.59</v>
+        <v>953.3</v>
       </c>
       <c r="D64" s="33" t="str">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO","A ser apurado",IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan","Insetkan","Apurado"))</f>
-        <v>Insetkan</v>
+        <v>A ser apurado</v>
       </c>
       <c r="E64" s="10">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO",0,IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan",0,Tabela1[[#This Row],[Faturar Após Medição]]))</f>
         <v>0</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>163</v>
+        <v>187</v>
       </c>
       <c r="G64" s="8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>158</v>
+        <v>109</v>
       </c>
       <c r="I64" s="7" t="s">
-        <v>155</v>
+        <v>65</v>
       </c>
       <c r="J64" s="7" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="K64" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="K64:K65" ca="1" si="1">IF(J64&gt;TODAY(),"Vigente","Encerrado")</f>
         <v>Vigente</v>
       </c>
-      <c r="L64" s="31" t="str">
+      <c r="L64" s="11" t="str">
         <f>VLOOKUP(Tabela1[[#This Row],[Chave]],'[1]07.2024'!$A$1:$P$70,15,0)</f>
-        <v>Insetkan</v>
+        <v>A ser apurado</v>
       </c>
       <c r="M64" s="7" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="N64" s="32" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
-        <v>INSET_Banco do Brasil_Controle de Pragas e Vetores</v>
+        <v>KT_Fundação Cultural do Exército Brasileiro - FUNCEB_Limpeza</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="32" t="s">
-        <v>166</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C65" s="10">
-        <v>4160.12</v>
-      </c>
-      <c r="D65" s="33" t="str">
+        <v>156</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C65" s="15">
+        <v>390.99</v>
+      </c>
+      <c r="D65" s="34" t="str">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO","A ser apurado",IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan","Insetkan","Apurado"))</f>
-        <v>Apurado</v>
-      </c>
-      <c r="E65" s="10">
-        <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO",0,IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan",0,Tabela1[[#This Row],[Faturar Após Medição]]))</f>
-        <v>4160.12</v>
-      </c>
-      <c r="F65" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="G65" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="H65" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="I65" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="J65" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="K65" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Vigente</v>
-      </c>
-      <c r="L65" s="11">
-        <f>VLOOKUP(Tabela1[[#This Row],[Chave]],'[1]07.2024'!$A$1:$P$70,15,0)</f>
-        <v>4160.12</v>
-      </c>
-      <c r="M65" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="N65" s="32" t="str">
-        <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
-        <v xml:space="preserve">KE_Banco da Providência_Limpeza </v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A66" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C66" s="10">
-        <v>2934.8</v>
-      </c>
-      <c r="D66" s="33" t="str">
-        <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO","A ser apurado",IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan","Insetkan","Apurado"))</f>
-        <v>Insetkan</v>
-      </c>
-      <c r="E66" s="10">
+        <v>A ser apurado</v>
+      </c>
+      <c r="E65" s="15">
         <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO",0,IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan",0,Tabela1[[#This Row],[Faturar Após Medição]]))</f>
         <v>0</v>
       </c>
-      <c r="F66" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="G66" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="H66" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="I66" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="J66" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="K66" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Vigente</v>
-      </c>
-      <c r="L66" s="31" t="str">
-        <f>VLOOKUP(Tabela1[[#This Row],[Chave]],'[1]07.2024'!$A$1:$P$70,15,0)</f>
-        <v>Insetkan</v>
-      </c>
-      <c r="M66" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="N66" s="32" t="str">
-        <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
-        <v>INSET_Serviço Social do Comércio - Polo Sociocultural Sesc Paraty_Controle de Pragas e Vetores</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A67" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="B67" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C67" s="10">
-        <v>2120</v>
-      </c>
-      <c r="D67" s="33" t="str">
-        <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO","A ser apurado",IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan","Insetkan","Apurado"))</f>
-        <v>Insetkan</v>
-      </c>
-      <c r="E67" s="10">
-        <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO",0,IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan",0,Tabela1[[#This Row],[Faturar Após Medição]]))</f>
-        <v>0</v>
-      </c>
-      <c r="F67" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="G67" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="H67" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="I67" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="J67" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="K67" s="9" t="str">
-        <f t="shared" ref="K67:K70" ca="1" si="1">IF(J67&gt;TODAY(),"Vigente","Encerrado")</f>
-        <v>Vigente</v>
-      </c>
-      <c r="L67" s="31" t="str">
-        <f>VLOOKUP(Tabela1[[#This Row],[Chave]],'[1]07.2024'!$A$1:$P$70,15,0)</f>
-        <v>Insetkan</v>
-      </c>
-      <c r="M67" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="N67" s="32" t="str">
-        <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
-        <v>INSET_Serviço Social do Comércio - Departamento Nacional_Controle de Pragas e Vetores</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A68" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="B68" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C68" s="10">
-        <v>1880</v>
-      </c>
-      <c r="D68" s="33" t="str">
-        <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO","A ser apurado",IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan","Insetkan","Apurado"))</f>
-        <v>Insetkan</v>
-      </c>
-      <c r="E68" s="10">
-        <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO",0,IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan",0,Tabela1[[#This Row],[Faturar Após Medição]]))</f>
-        <v>0</v>
-      </c>
-      <c r="F68" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="G68" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="H68" s="7">
-        <v>1574</v>
-      </c>
-      <c r="I68" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="J68" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="K68" s="9" t="str">
+      <c r="F65" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="G65" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="H65" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="I65" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="J65" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="K65" s="14" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>Vigente</v>
       </c>
-      <c r="L68" s="31" t="str">
-        <f>VLOOKUP(Tabela1[[#This Row],[Chave]],'[1]07.2024'!$A$1:$P$70,15,0)</f>
-        <v>Insetkan</v>
-      </c>
-      <c r="M68" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="N68" s="32" t="str">
-        <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
-        <v>INSET_Serviço Nacional de Aprendizagem Industrial - SENAI-CETIQT_Controle de Pragas e Vetores</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A69" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="B69" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C69" s="10">
-        <v>953.3</v>
-      </c>
-      <c r="D69" s="33" t="str">
-        <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO","A ser apurado",IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan","Insetkan","Apurado"))</f>
-        <v>A ser apurado</v>
-      </c>
-      <c r="E69" s="10">
-        <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO",0,IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan",0,Tabela1[[#This Row],[Faturar Após Medição]]))</f>
-        <v>0</v>
-      </c>
-      <c r="F69" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="G69" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="H69" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="I69" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="J69" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="K69" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Vigente</v>
-      </c>
-      <c r="L69" s="11" t="str">
+      <c r="L65" s="16" t="str">
         <f>VLOOKUP(Tabela1[[#This Row],[Chave]],'[1]07.2024'!$A$1:$P$70,15,0)</f>
         <v>A ser apurado</v>
       </c>
-      <c r="M69" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="N69" s="32" t="str">
-        <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
-        <v>KT_Fundação Cultural do Exército Brasileiro - FUNCEB_Limpeza</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A70" s="32" t="s">
-        <v>166</v>
-      </c>
-      <c r="B70" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C70" s="15">
-        <v>390.99</v>
-      </c>
-      <c r="D70" s="34" t="str">
-        <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO","A ser apurado",IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan","Insetkan","Apurado"))</f>
-        <v>A ser apurado</v>
-      </c>
-      <c r="E70" s="15">
-        <f>IF(Tabela1[[#This Row],[Faturar Após Medição]]="A SER APURADO",0,IF(Tabela1[[#This Row],[Faturar Após Medição]]="insetkan",0,Tabela1[[#This Row],[Faturar Após Medição]]))</f>
-        <v>0</v>
-      </c>
-      <c r="F70" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="G70" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="H70" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="I70" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="J70" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="K70" s="14" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Vigente</v>
-      </c>
-      <c r="L70" s="16" t="str">
-        <f>VLOOKUP(Tabela1[[#This Row],[Chave]],'[1]07.2024'!$A$1:$P$70,15,0)</f>
-        <v>A ser apurado</v>
-      </c>
-      <c r="M70" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="N70" s="40" t="str">
+      <c r="M65" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="N65" s="40" t="str">
         <f>Tabela1[[#This Row],[EMPR]]&amp;"_"&amp;Tabela1[[#This Row],[Razão Social do Tomador]]&amp;"_"&amp;Tabela1[[#This Row],[Objeto]]</f>
         <v>KE_Conferência Nacional dos Bispos do Brasil - CNBB_Limpeza Expressa</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <conditionalFormatting sqref="A2:K70">
+  <conditionalFormatting sqref="A2:K65">
     <cfRule type="expression" dxfId="1" priority="4">
       <formula>$M2="Encerrado"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L70 I71:I1048576">
+  <conditionalFormatting sqref="I66:I1048576 L1:L65">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="A ser apurado">
       <formula>NOT(ISERROR(SEARCH("A ser apurado",I1)))</formula>
     </cfRule>
@@ -8937,18 +8657,18 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1F18F452-72E2-41F2-BB8E-C375E17331F1}">
-          <x14:formula1>
-            <xm:f>Planilha2!$A$2:$A$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>G3:G70</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C888B976-EE8D-40D9-8ED3-8BBDBF9BDF75}">
           <x14:formula1>
             <xm:f>Planilha2!$A$2:$A$10</xm:f>
           </x14:formula1>
           <xm:sqref>G2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1F18F452-72E2-41F2-BB8E-C375E17331F1}">
+          <x14:formula1>
+            <xm:f>Planilha2!$A$2:$A$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>G3:G65</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -8971,47 +8691,47 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>